<commit_message>
20210518_updates QC control final PCAs before and after filtering expression inflammatory marker genes boxplots
</commit_message>
<xml_diff>
--- a/AD_analyses/data/multiqc_general.xlsx
+++ b/AD_analyses/data/multiqc_general.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Samsung_T5/MiG_data/MDD_microglia_analysis/MDD_microglia_analysis/AD_analyses/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4D926895-ED7C-044C-8769-7AB4A297433A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C74824D-8B13-664C-A4CE-16AB8D3165A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="980" windowWidth="27640" windowHeight="15520" xr2:uid="{7BCAA442-A8EC-2E4C-93D2-B721E78D7530}"/>
   </bookViews>
@@ -951,9 +951,6 @@
     <t>18-079-SVZ</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>18-105-GFM</t>
   </si>
   <si>
@@ -1042,6 +1039,9 @@
   </si>
   <si>
     <t>MG-14-SVZ</t>
+  </si>
+  <si>
+    <t>18-079-THA</t>
   </si>
 </sst>
 </file>
@@ -1438,8 +1438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5945F4BC-CE92-664C-AC2B-0566DAEFFAE4}">
   <dimension ref="A1:R315"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A265" workbookViewId="0">
+      <selection activeCell="A286" sqref="A286"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17350,7 +17350,7 @@
     </row>
     <row r="285" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A285" s="3" t="s">
-        <v>305</v>
+        <v>335</v>
       </c>
       <c r="B285" s="4">
         <v>21.202384987746299</v>
@@ -17406,7 +17406,7 @@
     </row>
     <row r="286" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A286" s="6" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B286" s="7">
         <v>32.138518929544396</v>
@@ -17462,7 +17462,7 @@
     </row>
     <row r="287" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A287" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B287" s="7">
         <v>11.6505031332252</v>
@@ -17518,7 +17518,7 @@
     </row>
     <row r="288" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A288" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B288" s="7">
         <v>40.138282646273296</v>
@@ -17574,7 +17574,7 @@
     </row>
     <row r="289" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A289" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B289" s="4">
         <v>76.2897181124372</v>
@@ -17630,7 +17630,7 @@
     </row>
     <row r="290" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A290" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B290" s="4">
         <v>72.764433405244105</v>
@@ -17686,7 +17686,7 @@
     </row>
     <row r="291" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A291" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B291" s="4">
         <v>7.8852323316737802</v>
@@ -17742,7 +17742,7 @@
     </row>
     <row r="292" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A292" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B292" s="4">
         <v>42.2331572023595</v>
@@ -17798,7 +17798,7 @@
     </row>
     <row r="293" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A293" s="3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B293" s="4">
         <v>41.100739795928199</v>
@@ -17854,7 +17854,7 @@
     </row>
     <row r="294" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A294" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B294" s="4">
         <v>65.109510077157097</v>
@@ -17910,7 +17910,7 @@
     </row>
     <row r="295" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A295" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B295" s="4">
         <v>42.325634860681902</v>
@@ -17966,7 +17966,7 @@
     </row>
     <row r="296" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A296" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B296" s="4">
         <v>10.273149067548299</v>
@@ -18022,7 +18022,7 @@
     </row>
     <row r="297" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A297" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B297" s="4">
         <v>9.6033574489236795</v>
@@ -18078,7 +18078,7 @@
     </row>
     <row r="298" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A298" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B298" s="4">
         <v>31.209944534744899</v>
@@ -18134,7 +18134,7 @@
     </row>
     <row r="299" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A299" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B299" s="4">
         <v>32.220321014933099</v>
@@ -18190,7 +18190,7 @@
     </row>
     <row r="300" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A300" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B300" s="4">
         <v>9.1525786055931402</v>
@@ -18246,7 +18246,7 @@
     </row>
     <row r="301" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A301" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B301" s="4">
         <v>10.846433681563299</v>
@@ -18302,7 +18302,7 @@
     </row>
     <row r="302" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A302" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B302" s="4">
         <v>13.681085326727199</v>
@@ -18358,7 +18358,7 @@
     </row>
     <row r="303" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A303" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B303" s="4">
         <v>16.701578754340101</v>
@@ -18414,7 +18414,7 @@
     </row>
     <row r="304" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A304" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B304" s="4">
         <v>27.897022567840299</v>
@@ -18470,7 +18470,7 @@
     </row>
     <row r="305" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A305" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B305" s="4">
         <v>38.713767423251198</v>
@@ -18526,7 +18526,7 @@
     </row>
     <row r="306" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A306" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B306" s="4">
         <v>43.073605319604397</v>
@@ -18582,7 +18582,7 @@
     </row>
     <row r="307" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A307" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B307" s="4">
         <v>48.330247930173002</v>
@@ -18638,7 +18638,7 @@
     </row>
     <row r="308" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A308" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B308" s="4">
         <v>21.898124348568398</v>
@@ -18694,7 +18694,7 @@
     </row>
     <row r="309" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A309" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B309" s="4">
         <v>27.133332950943899</v>
@@ -18750,7 +18750,7 @@
     </row>
     <row r="310" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A310" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B310" s="4">
         <v>41.178306315633598</v>
@@ -18806,7 +18806,7 @@
     </row>
     <row r="311" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A311" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B311" s="4">
         <v>36.472459586853098</v>
@@ -18862,7 +18862,7 @@
     </row>
     <row r="312" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A312" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B312" s="4">
         <v>11.587386569589301</v>
@@ -18918,7 +18918,7 @@
     </row>
     <row r="313" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A313" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B313" s="4">
         <v>12.005259788308299</v>
@@ -18974,7 +18974,7 @@
     </row>
     <row r="314" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A314" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B314" s="4">
         <v>15.5936260966334</v>
@@ -19030,7 +19030,7 @@
     </row>
     <row r="315" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A315" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B315" s="4">
         <v>5.5461757067992696</v>

</xml_diff>